<commit_message>
feat: load of events done
</commit_message>
<xml_diff>
--- a/excelDatos/EventData.xlsx
+++ b/excelDatos/EventData.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26924"/>
+  <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\caja_fuerte\programar\universidad\sexto_semestre\proyecto_integrador_I\icesi-filantrop-a-equipo-4\excelDatos\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A9FA2E8-4634-425F-AF4A-B94235072DEB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -18,8 +24,67 @@
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+  <si>
+    <t>name</t>
+  </si>
+  <si>
+    <t>date</t>
+  </si>
+  <si>
+    <t>event_type</t>
+  </si>
+  <si>
+    <t>time</t>
+  </si>
+  <si>
+    <t>sponsor_name</t>
+  </si>
+  <si>
+    <t>participation</t>
+  </si>
+  <si>
+    <t>desayuno con COLGATE</t>
+  </si>
+  <si>
+    <t>F</t>
+  </si>
+  <si>
+    <t>O</t>
+  </si>
+  <si>
+    <t>COLGATE</t>
+  </si>
+  <si>
+    <t>desayuno con representate de colgate</t>
+  </si>
+  <si>
+    <t>Reunion de control</t>
+  </si>
+  <si>
+    <t>2023-10-03</t>
+  </si>
+  <si>
+    <t>2024-01-07</t>
+  </si>
+  <si>
+    <t>08:30:00</t>
+  </si>
+  <si>
+    <t>16:45:00</t>
+  </si>
+  <si>
+    <t>LAURA MEDINA</t>
+  </si>
+  <si>
+    <t>control de calidad</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -49,8 +114,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -330,13 +396,85 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:F3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D4" sqref="D4"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="21.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="35.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E3" t="s">
+        <v>16</v>
+      </c>
+      <c r="F3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
fix: more examples added
</commit_message>
<xml_diff>
--- a/excelDatos/EventData.xlsx
+++ b/excelDatos/EventData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\caja_fuerte\programar\universidad\sexto_semestre\proyecto_integrador_I\icesi-filantrop-a-equipo-4\excelDatos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A9FA2E8-4634-425F-AF4A-B94235072DEB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3EA70EC4-CC08-4B78-9B71-118AB10075A3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="14295" yWindow="0" windowWidth="14610" windowHeight="15585" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="32">
   <si>
     <t>name</t>
   </si>
@@ -79,6 +79,48 @@
   </si>
   <si>
     <t>control de calidad</t>
+  </si>
+  <si>
+    <t>almuerzo con DELL</t>
+  </si>
+  <si>
+    <t>DELL</t>
+  </si>
+  <si>
+    <t>ESTEBAN GUTIERREZ</t>
+  </si>
+  <si>
+    <t>PEPSI</t>
+  </si>
+  <si>
+    <t>ANDRES GOMEZ</t>
+  </si>
+  <si>
+    <t>MICROSOFT</t>
+  </si>
+  <si>
+    <t>patrocinador del almuerzo</t>
+  </si>
+  <si>
+    <t>pago para estudientes</t>
+  </si>
+  <si>
+    <t>revicion de notas estudientes becados</t>
+  </si>
+  <si>
+    <t>desayuno con Andres Gomez</t>
+  </si>
+  <si>
+    <t>reparto de equipos</t>
+  </si>
+  <si>
+    <t>entrega de material Microsoft</t>
+  </si>
+  <si>
+    <t>reunion de control estudientes</t>
+  </si>
+  <si>
+    <t>recaudo becas</t>
   </si>
 </sst>
 </file>
@@ -397,19 +439,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F3"/>
+  <dimension ref="A1:F8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="21.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="27.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="11.140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10.7109375" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="8.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="18.85546875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="35.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -473,6 +515,76 @@
         <v>17</v>
       </c>
     </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>18</v>
+      </c>
+      <c r="B4" t="s">
+        <v>8</v>
+      </c>
+      <c r="E4" t="s">
+        <v>19</v>
+      </c>
+      <c r="F4" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>31</v>
+      </c>
+      <c r="B5" t="s">
+        <v>7</v>
+      </c>
+      <c r="E5" t="s">
+        <v>20</v>
+      </c>
+      <c r="F5" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>30</v>
+      </c>
+      <c r="B6" t="s">
+        <v>8</v>
+      </c>
+      <c r="E6" t="s">
+        <v>21</v>
+      </c>
+      <c r="F6" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>27</v>
+      </c>
+      <c r="B7" t="s">
+        <v>7</v>
+      </c>
+      <c r="E7" t="s">
+        <v>22</v>
+      </c>
+      <c r="F7" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>29</v>
+      </c>
+      <c r="B8" t="s">
+        <v>7</v>
+      </c>
+      <c r="E8" t="s">
+        <v>23</v>
+      </c>
+      <c r="F8" t="s">
+        <v>28</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>

</xml_diff>